<commit_message>
Changes to data storage, and rectangle drawing feature added.
</commit_message>
<xml_diff>
--- a/base/SynonymBook.xlsx
+++ b/base/SynonymBook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scg2600\OneDrive - University of Texas at Arlington\Documents\eeCarbonVisualization3\base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/sean_guidrystanteen_mavs_uta_edu/Documents/Documents/eeCarbonVisualization3/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1769B07-6227-4173-B9C6-2B3E0DADF302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{CEFC2612-4D2A-4E10-B4F2-191626252F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9345877D-F649-435E-B9D7-53CF7B800A5B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{784D41EA-42FF-4002-9C28-AAAC6409EF92}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{784D41EA-42FF-4002-9C28-AAAC6409EF92}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="122">
   <si>
     <t>ISCN</t>
   </si>
@@ -94,21 +94,9 @@
     <t>SOC_pred1</t>
   </si>
   <si>
-    <t>layer_top (cm)</t>
-  </si>
-  <si>
-    <t>layer_bot (cm)</t>
-  </si>
-  <si>
     <t>layer_name</t>
   </si>
   <si>
-    <t>bd_samp (g cm-3)</t>
-  </si>
-  <si>
-    <t>soc (g cm-2)</t>
-  </si>
-  <si>
     <t>profile_name</t>
   </si>
   <si>
@@ -316,15 +304,6 @@
     <t>Texture Class</t>
   </si>
   <si>
-    <t>sand_tot_psa</t>
-  </si>
-  <si>
-    <t>silt_tot_psa</t>
-  </si>
-  <si>
-    <t>clay_tot_psa</t>
-  </si>
-  <si>
     <t>Splinable</t>
   </si>
   <si>
@@ -341,6 +320,90 @@
   </si>
   <si>
     <t>The value to distinguish between alike Pedons</t>
+  </si>
+  <si>
+    <t>lat_dec._deg</t>
+  </si>
+  <si>
+    <t>long_dec._deg</t>
+  </si>
+  <si>
+    <t>silt_tot_psa_percent</t>
+  </si>
+  <si>
+    <t>clay_tot_psa_percent</t>
+  </si>
+  <si>
+    <t>sand_tot_psa_percent</t>
+  </si>
+  <si>
+    <t>layer_top_cm</t>
+  </si>
+  <si>
+    <t>layer_bot_cm</t>
+  </si>
+  <si>
+    <t>soc_g_cm-2</t>
+  </si>
+  <si>
+    <t>bd_samp_g_cm-3</t>
+  </si>
+  <si>
+    <t>S3C</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>S3C0</t>
+  </si>
+  <si>
+    <t>pedkey</t>
+  </si>
+  <si>
+    <t>idped</t>
+  </si>
+  <si>
+    <t>idsam</t>
+  </si>
+  <si>
+    <t>oc</t>
+  </si>
+  <si>
+    <t>sand</t>
+  </si>
+  <si>
+    <t>silt</t>
+  </si>
+  <si>
+    <t>clay</t>
+  </si>
+  <si>
+    <t>bd3</t>
+  </si>
+  <si>
+    <t>thdep</t>
+  </si>
+  <si>
+    <t>thbot</t>
+  </si>
+  <si>
+    <t>S3C1</t>
+  </si>
+  <si>
+    <t>dlat</t>
+  </si>
+  <si>
+    <t>dlong</t>
+  </si>
+  <si>
+    <t>s3c_v20040427 ,TABLE, horiz01</t>
+  </si>
+  <si>
+    <t>ACCESS</t>
+  </si>
+  <si>
+    <t>s3c_v20040427 ,TABLE, pedon01</t>
   </si>
 </sst>
 </file>
@@ -405,9 +468,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42DBD29B-DEDE-4B44-82D4-E79896288EEF}" name="Table1" displayName="Table1" ref="A1:F43" totalsRowShown="0">
-  <autoFilter ref="A1:F43" xr:uid="{42DBD29B-DEDE-4B44-82D4-E79896288EEF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42DBD29B-DEDE-4B44-82D4-E79896288EEF}" name="Table1" displayName="Table1" ref="A1:F62" totalsRowShown="0">
+  <autoFilter ref="A1:F62" xr:uid="{42DBD29B-DEDE-4B44-82D4-E79896288EEF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F39">
     <sortCondition descending="1" ref="D1:D39"/>
   </sortState>
@@ -734,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1475E37-6C03-4EA5-926F-71652625F67D}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,22 +817,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -776,115 +843,115 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -895,13 +962,13 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -909,7 +976,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -918,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -926,7 +993,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -935,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -943,16 +1010,16 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -960,16 +1027,16 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -977,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -986,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -994,16 +1061,16 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1011,16 +1078,16 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1028,58 +1095,58 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -1088,15 +1155,15 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1105,49 +1172,49 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
@@ -1156,15 +1223,15 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -1173,49 +1240,49 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
@@ -1224,12 +1291,12 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
@@ -1241,12 +1308,12 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -1258,12 +1325,12 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
@@ -1275,12 +1342,12 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
         <v>14</v>
@@ -1292,46 +1359,46 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
         <v>16</v>
@@ -1343,92 +1410,92 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1436,16 +1503,16 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1453,16 +1520,16 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1470,16 +1537,339 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
         <v>94</v>
       </c>
-      <c r="C43" t="s">
-        <v>89</v>
-      </c>
-      <c r="D43" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" t="s">
-        <v>78</v>
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" t="b">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" t="s">
+        <v>62</v>
+      </c>
+      <c r="D52" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60" t="b">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>103</v>
+      </c>
+      <c r="B61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1492,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0755E869-BC02-4601-BB04-2CA8A4C75850}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1518,55 +1908,55 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1574,58 +1964,86 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1640,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C248E7-9B7D-44EC-9BE9-8A8D9A336DB1}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1653,19 +2071,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1679,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1721,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1735,12 +2153,12 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1760,7 +2178,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1774,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1788,12 +2206,12 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
@@ -1804,7 +2222,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
@@ -1815,7 +2233,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
@@ -1824,12 +2242,12 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
@@ -1838,12 +2256,12 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B15" t="b">
         <v>0</v>
@@ -1852,12 +2270,12 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B16" t="b">
         <v>0</v>
@@ -1866,12 +2284,12 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
@@ -1882,7 +2300,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
@@ -1893,7 +2311,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
@@ -1904,7 +2322,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -1915,7 +2333,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -1926,7 +2344,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B22" t="b">
         <v>1</v>
@@ -1937,7 +2355,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Last minute upload before update
</commit_message>
<xml_diff>
--- a/base/SynonymBook.xlsx
+++ b/base/SynonymBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mavsuta-my.sharepoint.com/personal/sean_guidrystanteen_mavs_uta_edu/Documents/Documents/eeCarbonVisualization3/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{CEFC2612-4D2A-4E10-B4F2-191626252F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9345877D-F649-435E-B9D7-53CF7B800A5B}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{56C884B1-FE1E-4945-BDBD-9256DE5E6BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C7E661C-B6BA-45B1-AC21-7A1544A8E6B3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{784D41EA-42FF-4002-9C28-AAAC6409EF92}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{784D41EA-42FF-4002-9C28-AAAC6409EF92}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="124">
   <si>
     <t>ISCN</t>
   </si>
@@ -404,6 +404,12 @@
   </si>
   <si>
     <t>s3c_v20040427 ,TABLE, pedon01</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>County</t>
   </si>
 </sst>
 </file>
@@ -475,8 +481,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42DBD29B-DEDE-4B44-82D4-E79896288EEF}" name="Table1" displayName="Table1" ref="A1:F62" totalsRowShown="0">
   <autoFilter ref="A1:F62" xr:uid="{42DBD29B-DEDE-4B44-82D4-E79896288EEF}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F39">
-    <sortCondition descending="1" ref="D1:D39"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F62">
+    <sortCondition ref="E1:E62"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{FF56D98B-6522-441D-8747-CE5441F2ABC1}" name="Source"/>
@@ -491,8 +497,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{717DCF6C-22D6-492F-BFA9-68DC5C9E4DE2}" name="Table3" displayName="Table3" ref="A1:E23" totalsRowShown="0">
-  <autoFilter ref="A1:E23" xr:uid="{717DCF6C-22D6-492F-BFA9-68DC5C9E4DE2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{717DCF6C-22D6-492F-BFA9-68DC5C9E4DE2}" name="Table3" displayName="Table3" ref="A1:E25" totalsRowShown="0">
+  <autoFilter ref="A1:E25" xr:uid="{717DCF6C-22D6-492F-BFA9-68DC5C9E4DE2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{E58916E2-01B8-4D2B-8B3E-8967F9B0C5A2}" name="Standard"/>
     <tableColumn id="2" xr3:uid="{0FDA8C46-CAF8-4DFC-923B-A561B51BB8ED}" name="Splinable"/>
@@ -803,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1475E37-6C03-4EA5-926F-71652625F67D}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="M61" sqref="M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,104 +860,104 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>62</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -959,10 +965,10 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -976,10 +982,10 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -993,10 +999,10 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1010,10 +1016,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1027,10 +1033,10 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -1044,10 +1050,10 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -1061,10 +1067,10 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1078,10 +1084,10 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -1095,10 +1101,10 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -1112,13 +1118,13 @@
         <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>70</v>
@@ -1129,10 +1135,10 @@
         <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -1146,10 +1152,10 @@
         <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -1163,10 +1169,10 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -1180,16 +1186,16 @@
         <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1197,13 +1203,13 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="s">
         <v>71</v>
@@ -1214,10 +1220,10 @@
         <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -1231,10 +1237,10 @@
         <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -1248,16 +1254,16 @@
         <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1265,16 +1271,16 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1282,84 +1288,84 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="D28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1367,16 +1373,16 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1384,16 +1390,16 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1401,16 +1407,16 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1418,13 +1424,13 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
         <v>76</v>
@@ -1435,10 +1441,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -1452,10 +1458,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
@@ -1469,10 +1475,10 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -1486,10 +1492,10 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -1500,121 +1506,121 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="C46" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1628,7 +1634,7 @@
         <v>61</v>
       </c>
       <c r="D48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" t="s">
         <v>105</v>
@@ -1656,10 +1662,10 @@
         <v>103</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
@@ -1673,10 +1679,10 @@
         <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C51" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
@@ -1690,10 +1696,10 @@
         <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C52" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -1707,10 +1713,10 @@
         <v>103</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -1724,10 +1730,10 @@
         <v>103</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C54" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -1741,10 +1747,10 @@
         <v>103</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C55" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -1758,10 +1764,10 @@
         <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C56" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -1775,10 +1781,10 @@
         <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C57" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -1792,10 +1798,10 @@
         <v>103</v>
       </c>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -1809,16 +1815,16 @@
         <v>103</v>
       </c>
       <c r="B59" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="D59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1832,7 +1838,7 @@
         <v>81</v>
       </c>
       <c r="D60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" t="s">
         <v>116</v>
@@ -1884,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0755E869-BC02-4601-BB04-2CA8A4C75850}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2056,10 +2062,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C248E7-9B7D-44EC-9BE9-8A8D9A336DB1}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2364,6 +2370,28 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>